<commit_message>
lots of file updates for inputs for tme experiment and corresponding code updates in Rmd file
</commit_message>
<xml_diff>
--- a/data/derived/air-dry-2019-whc/air-dry-2019-whc_2020-04-21.xlsx
+++ b/data/derived/air-dry-2019-whc/air-dry-2019-whc_2020-04-21.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="24880" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="24880" windowHeight="16740" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -701,7 +701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1880,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1906,8 +1906,8 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="str">
-        <f>IF(WHC!A5="Field","control (2019)","air-dry (2019")</f>
-        <v>control (2019)</v>
+        <f>IF(WHC!A5="Field","control","air-dry")</f>
+        <v>control</v>
       </c>
       <c r="B2" t="str">
         <f>WHC!B5</f>
@@ -1924,8 +1924,8 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="str">
-        <f>IF(WHC!A6="Field","control (2019)","air-dry (2019")</f>
-        <v>control (2019)</v>
+        <f>IF(WHC!A6="Field","control","air-dry")</f>
+        <v>control</v>
       </c>
       <c r="B3" t="str">
         <f>WHC!B6</f>
@@ -1942,8 +1942,8 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="str">
-        <f>IF(WHC!A7="Field","control (2019)","air-dry (2019")</f>
-        <v>control (2019)</v>
+        <f>IF(WHC!A7="Field","control","air-dry")</f>
+        <v>control</v>
       </c>
       <c r="B4" t="str">
         <f>WHC!B7</f>
@@ -1960,8 +1960,8 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="str">
-        <f>IF(WHC!A8="Field","control (2019)","air-dry (2019")</f>
-        <v>control (2019)</v>
+        <f>IF(WHC!A8="Field","control","air-dry")</f>
+        <v>control</v>
       </c>
       <c r="B5" t="str">
         <f>WHC!B8</f>
@@ -1978,8 +1978,8 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="str">
-        <f>IF(WHC!A9="Field","control (2019)","air-dry (2019")</f>
-        <v>control (2019)</v>
+        <f>IF(WHC!A9="Field","control","air-dry")</f>
+        <v>control</v>
       </c>
       <c r="B6" t="str">
         <f>WHC!B9</f>
@@ -1996,8 +1996,8 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="str">
-        <f>IF(WHC!A10="Field","control (2019)","air-dry (2019")</f>
-        <v>control (2019)</v>
+        <f>IF(WHC!A10="Field","control","air-dry")</f>
+        <v>control</v>
       </c>
       <c r="B7" t="str">
         <f>WHC!B10</f>
@@ -2014,8 +2014,8 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="str">
-        <f>IF(WHC!A11="Field","control (2019)","air-dry (2019)")</f>
-        <v>air-dry (2019)</v>
+        <f>IF(WHC!A11="Field","control","air-dry")</f>
+        <v>air-dry</v>
       </c>
       <c r="B8" t="str">
         <f>WHC!B11</f>
@@ -2032,8 +2032,8 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="str">
-        <f>IF(WHC!A12="Field","control (2019)","air-dry (2019)")</f>
-        <v>air-dry (2019)</v>
+        <f>IF(WHC!A12="Field","control","air-dry")</f>
+        <v>air-dry</v>
       </c>
       <c r="B9" t="str">
         <f>WHC!B12</f>
@@ -2050,8 +2050,8 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="str">
-        <f>IF(WHC!A13="Field","control (2019)","air-dry (2019)")</f>
-        <v>air-dry (2019)</v>
+        <f>IF(WHC!A13="Field","control","air-dry")</f>
+        <v>air-dry</v>
       </c>
       <c r="B10" t="str">
         <f>WHC!B13</f>
@@ -2068,8 +2068,8 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="str">
-        <f>IF(WHC!A14="Field","control (2019)","air-dry (2019)")</f>
-        <v>air-dry (2019)</v>
+        <f>IF(WHC!A14="Field","control","air-dry")</f>
+        <v>air-dry</v>
       </c>
       <c r="B11" t="str">
         <f>WHC!B14</f>
@@ -2086,8 +2086,8 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="str">
-        <f>IF(WHC!A15="Field","control (2019)","air-dry (2019)")</f>
-        <v>air-dry (2019)</v>
+        <f>IF(WHC!A15="Field","control","air-dry")</f>
+        <v>air-dry</v>
       </c>
       <c r="B12" t="str">
         <f>WHC!B15</f>
@@ -2104,8 +2104,8 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="str">
-        <f>IF(WHC!A16="Field","control (2019)","air-dry (2019)")</f>
-        <v>air-dry (2019)</v>
+        <f>IF(WHC!A16="Field","control","air-dry")</f>
+        <v>air-dry</v>
       </c>
       <c r="B13" t="str">
         <f>WHC!B16</f>

</xml_diff>